<commit_message>
Change over from v1.0.1 to v1.1.0
</commit_message>
<xml_diff>
--- a/input/fsh/scripts/carin-bb-server.xlsx
+++ b/input/fsh/scripts/carin-bb-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git-alt/MyNotebooks/CapStatement/temp_source_spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\FHIR\FSH\DaVinciIG_Dev\CARINBB\carin-bb\input\fsh\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDD04B8-9938-9E41-BA5B-6B55078B3374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A38C44-8F59-4B1E-81C8-31E2E5BC4DD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="2020" windowWidth="64520" windowHeight="25180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2025" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -458,9 +458,6 @@
     <t>fhirVersion</t>
   </si>
   <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
     <t>pre</t>
   </si>
   <si>
@@ -710,12 +707,15 @@
 1. Support xml source formats for all C4BB interactions.
 </t>
   </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1291,12 +1291,12 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="61.83203125" customWidth="1"/>
+    <col min="2" max="2" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1304,103 +1304,103 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="12" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1419,21 +1419,21 @@
       <selection activeCell="A2" sqref="A2:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="96.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="88.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="82.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="96.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="88.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="82.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -1465,50 +1465,50 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="82" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="81.95" customHeight="1" thickTop="1">
       <c r="C2" s="30"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="C3" s="30"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="C4" s="30"/>
       <c r="E4"/>
       <c r="F4"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="C5" s="30"/>
       <c r="E5"/>
       <c r="F5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="C6" s="30"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="C7" s="30"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="C8" s="30"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="C9" s="30"/>
       <c r="E9"/>
       <c r="F9"/>
@@ -1516,335 +1516,335 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="C10" s="30"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="H10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="C11" s="30"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="C12" s="30"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="H12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="1" customFormat="1">
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="1" customFormat="1">
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="8:10">
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="8:10" s="1" customFormat="1">
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="8:10" s="1" customFormat="1">
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="8:10" s="1" customFormat="1">
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="8:10">
       <c r="H21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="8:10" s="1" customFormat="1">
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="8:10" s="1" customFormat="1">
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="8:10" s="1" customFormat="1">
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="8:10" s="1" customFormat="1">
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="8:10" s="1" customFormat="1">
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="8:10" s="1" customFormat="1">
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="8:10" s="1" customFormat="1">
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="8:10" s="1" customFormat="1">
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="8:10" s="1" customFormat="1">
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="8:10" s="1" customFormat="1">
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="8:10" s="1" customFormat="1">
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:10" s="1" customFormat="1">
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:10" s="1" customFormat="1">
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:10" s="1" customFormat="1">
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:10" s="1" customFormat="1">
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:10" s="1" customFormat="1">
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:10" s="1" customFormat="1">
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:10" s="1" customFormat="1">
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:10" s="1" customFormat="1" ht="15.75">
       <c r="H40" s="5"/>
       <c r="I40" s="7"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:10" s="1" customFormat="1" ht="15.75">
       <c r="H41" s="5"/>
       <c r="I41" s="7"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:10" s="1" customFormat="1" ht="15.75">
       <c r="H42" s="5"/>
       <c r="I42" s="7"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:10" s="1" customFormat="1">
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:10" s="1" customFormat="1">
       <c r="C44" s="9"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:10" s="1" customFormat="1">
       <c r="C45" s="9"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:10" s="1" customFormat="1">
       <c r="C46" s="9"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:10" s="1" customFormat="1">
       <c r="C47" s="9"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:10" s="1" customFormat="1">
       <c r="C48" s="9"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:10" s="1" customFormat="1">
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:10" s="1" customFormat="1">
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:10" s="1" customFormat="1">
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:10" s="1" customFormat="1">
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:10" s="1" customFormat="1">
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:10" s="1" customFormat="1">
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:10" s="1" customFormat="1">
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:10" s="1" customFormat="1">
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:10" s="1" customFormat="1">
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:10" s="1" customFormat="1">
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:10" s="1" customFormat="1">
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:10" s="1" customFormat="1">
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:10" s="1" customFormat="1">
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:10" s="1" customFormat="1">
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:10" s="1" customFormat="1">
       <c r="C63" s="9"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:10" s="1" customFormat="1">
       <c r="C64" s="9"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:16" s="1" customFormat="1">
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:16" s="1" customFormat="1">
       <c r="C66" s="9"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:16" s="1" customFormat="1">
       <c r="C67" s="9"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:16" s="1" customFormat="1">
       <c r="C68" s="9"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:16" s="1" customFormat="1">
       <c r="C69" s="9"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:16" s="1" customFormat="1">
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" spans="3:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:16" s="1" customFormat="1" ht="15.75">
       <c r="C71" s="8"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:16" s="1" customFormat="1">
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:16" s="1" customFormat="1">
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:16" s="1" customFormat="1">
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:16" s="1" customFormat="1">
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:16">
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
@@ -1855,37 +1855,37 @@
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
     </row>
-    <row r="77" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:16" s="1" customFormat="1">
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1">
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:16" s="1" customFormat="1">
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1">
       <c r="H80" s="5"/>
       <c r="I80" s="7"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="8:10" s="1" customFormat="1">
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="8:10" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="8:10" s="1" customFormat="1" ht="20.25" customHeight="1">
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
     </row>
-    <row r="83" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="8:10" s="1" customFormat="1">
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
@@ -1903,17 +1903,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1921,55 +1921,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="15.75">
       <c r="A3" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="257" customHeight="1" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="257.10000000000002" customHeight="1">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1977,20 +1977,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="351.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="351.75" customHeight="1">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="103.5" customHeight="1">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2009,9 +2009,9 @@
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2032,15 +2032,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="114.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="114.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="27" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="27" customFormat="1" ht="23.25">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -2054,122 +2054,122 @@
         <v>12</v>
       </c>
       <c r="E1" s="27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="18.75">
+      <c r="A2" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="3" spans="1:6" ht="18.75">
+      <c r="A3" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>176</v>
-      </c>
       <c r="B3" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18.75">
       <c r="A4" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="18.75">
       <c r="A5" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="18.75">
       <c r="A6" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E6" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="18.75">
       <c r="A7" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18.75">
       <c r="A8" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>13</v>
@@ -2182,12 +2182,12 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="18.75">
       <c r="A9" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>13</v>
@@ -2200,12 +2200,12 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="18.75">
       <c r="A10" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>13</v>
@@ -2238,22 +2238,22 @@
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="25.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
-    <col min="5" max="12" width="17.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5" style="1" customWidth="1"/>
-    <col min="14" max="17" width="17.5" style="1" customWidth="1"/>
-    <col min="18" max="19" width="20.5" style="1" customWidth="1"/>
-    <col min="20" max="20" width="36.6640625" style="2" customWidth="1"/>
-    <col min="21" max="23" width="38.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="72.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="5" max="12" width="17.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" style="1" customWidth="1"/>
+    <col min="14" max="17" width="17.42578125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="20.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="36.7109375" style="2" customWidth="1"/>
+    <col min="21" max="23" width="38.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="72.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="25.5" customHeight="1" thickBot="1">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2327,9 +2327,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="21" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="19.5" thickTop="1">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -2343,21 +2343,21 @@
         <v>13</v>
       </c>
       <c r="T2" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V2" s="20"/>
       <c r="W2" s="20"/>
       <c r="X2"/>
     </row>
-    <row r="3" spans="1:24" ht="305" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="315">
       <c r="A3" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>21</v>
@@ -2366,11 +2366,11 @@
         <v>13</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="W3" s="20"/>
     </row>
-    <row r="4" spans="1:24" ht="16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
@@ -2386,7 +2386,7 @@
       <c r="V4" s="20"/>
       <c r="W4" s="20"/>
     </row>
-    <row r="5" spans="1:24" ht="16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="V5" s="20"/>
       <c r="W5" s="20"/>
     </row>
-    <row r="6" spans="1:24" ht="16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2417,18 +2417,18 @@
       </c>
       <c r="W6" s="20"/>
     </row>
-    <row r="7" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" ht="25.5" customHeight="1">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="25.5" customHeight="1">
       <c r="A8"/>
     </row>
-    <row r="39" spans="20:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="20:23" ht="25.5" customHeight="1">
       <c r="T39" s="21"/>
       <c r="V39" s="21"/>
       <c r="W39" s="21"/>
     </row>
-    <row r="42" spans="20:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="20:23" ht="25.5" customHeight="1">
       <c r="W42" s="21"/>
     </row>
   </sheetData>
@@ -2449,15 +2449,15 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="E2" s="2"/>
     </row>
   </sheetData>
@@ -2493,30 +2493,30 @@
       <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>90</v>
@@ -2525,16 +2525,16 @@
         <v>91</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2543,7 +2543,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2552,7 +2552,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="180">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2560,20 +2560,20 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>63</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>63</v>
@@ -2602,7 +2602,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -2611,7 +2611,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -2620,7 +2620,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -2629,7 +2629,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2638,7 +2638,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2647,7 +2647,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
       <c r="H12" s="1"/>
@@ -2666,13 +2666,13 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="51.1640625" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -2683,28 +2683,28 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="59.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>110</v>
       </c>
@@ -2727,38 +2727,38 @@
       <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="43" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="75.5" style="31" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
-    <col min="9" max="9" width="23.5" customWidth="1"/>
-    <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="75.42578125" style="31" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="15" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" style="1" customWidth="1"/>
     <col min="20" max="20" width="15" style="1" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.83203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" style="1" customWidth="1"/>
     <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="38.33203125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="24.33203125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="38.1640625" customWidth="1"/>
+    <col min="24" max="24" width="50.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="38.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="24.28515625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="18" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="13" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" s="13" customFormat="1" ht="15.75" thickTop="1">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" s="13" customFormat="1" ht="15">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" s="13" customFormat="1" ht="15">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="13" customFormat="1" ht="61" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="13" customFormat="1" ht="72">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" s="13" customFormat="1" ht="15">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" s="13" customFormat="1" ht="15">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" s="13" customFormat="1" ht="15">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -3183,15 +3183,15 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="65" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="96">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -3200,13 +3200,13 @@
         <v>1</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G9" t="s">
         <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I9" t="s">
         <v>58</v>
@@ -3230,13 +3230,13 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-_id.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="65" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="96">
       <c r="A10" s="1">
         <f>A9+1</f>
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>68</v>
@@ -3248,7 +3248,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G10" t="s">
         <v>57</v>
@@ -3284,16 +3284,16 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="65" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="96">
       <c r="A11" s="1">
         <f t="shared" ref="A11:A19" si="9">A10+1</f>
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -3302,13 +3302,13 @@
         <v>1</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G11" t="s">
         <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>64</v>
@@ -3336,13 +3336,13 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-_lastupdated.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="65" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="96">
       <c r="A12" s="1">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>14</v>
@@ -3354,7 +3354,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G12" t="s">
         <v>57</v>
@@ -3385,16 +3385,16 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-type.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" s="1" customFormat="1" ht="96">
       <c r="A13" s="1">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -3403,7 +3403,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>57</v>
@@ -3434,16 +3434,16 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-identifier.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="65" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="96">
       <c r="A14" s="1">
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -3452,7 +3452,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G14" t="s">
         <v>57</v>
@@ -3483,16 +3483,16 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-service-date.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="96">
       <c r="A15" s="1">
         <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -3501,7 +3501,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>57</v>
@@ -3539,16 +3539,16 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-provider.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" s="1" customFormat="1" ht="96">
       <c r="A16" s="1">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -3557,7 +3557,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>57</v>
@@ -3595,16 +3595,16 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-care-team.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" s="1" customFormat="1" ht="96">
       <c r="A17" s="1">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -3613,7 +3613,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>57</v>
@@ -3651,16 +3651,16 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-insurer.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" s="1" customFormat="1" ht="96">
       <c r="A18" s="1">
         <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
@@ -3669,7 +3669,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
@@ -3707,16 +3707,16 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-facility.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" s="1" customFormat="1" ht="96">
       <c r="A19" s="1">
         <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -3725,7 +3725,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>57</v>
@@ -3763,16 +3763,16 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-coverage.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="18.95" customHeight="1">
       <c r="A20" s="1">
         <f>A19+1</f>
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -3781,13 +3781,13 @@
         <v>1</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>57</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>58</v>
@@ -3811,68 +3811,68 @@
         <v>SearchParameter-carin-bb-!coverage-_id.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="F21" s="31"/>
       <c r="Y21" s="17"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="18.95" customHeight="1">
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="Y22" s="17"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="18.95" customHeight="1">
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="Y23" s="17"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="18.95" customHeight="1">
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="Y24" s="17"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="18.95" customHeight="1">
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="Y25" s="17"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="18.95" customHeight="1">
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="Y26" s="17"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="18.95" customHeight="1">
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="Y27" s="17"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="18.95" customHeight="1">
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="Y28" s="17"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="18.95" customHeight="1">
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="Y29" s="17"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="18.95" customHeight="1">
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>

</xml_diff>

<commit_message>
Peer Review version number change to 1.0.9
</commit_message>
<xml_diff>
--- a/input/fsh/scripts/carin-bb-server.xlsx
+++ b/input/fsh/scripts/carin-bb-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\FHIR\FSH\DaVinciIG_Dev\CARINBB\carin-bb\input\fsh\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF7B8EC-D207-4EDE-816B-A3DE20720FA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60803F8-2CEE-44D3-9DA3-06A5913D0E9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2025" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -696,9 +696,6 @@
 </t>
   </si>
   <si>
-    <t>1.1.0</t>
-  </si>
-  <si>
     <t>../../../output\us-core-comparisons/spec.internals</t>
   </si>
   <si>
@@ -709,6 +706,9 @@
     <t>This Section describes the expected capabilities of the C4BB Server actor which is responsible for providing responses to the queries submitted by the C4BB Requestors. 
 The EOB Resource is the focal Consumer-Directed Payer Data Exchange (CDPDE) Resource. Several Reference Resources are defined directly/indirectly from the EOB: Coverage, Patient, Organization (Payer ID), Practioner, and Organization (Facility).
 The Coverage Reference Resource SHALL be returned with data that was effective as of the date of service of the claim; for example, the data will reflect the employer name in effect at that time. However, for other reference resources, payers MAY decide to provide either the data that was in effect as of the date of service or the current data. All reference resources within the EOB will have meta.lastUpdated flagged as must support. Payers SHALL provide the last time the data was updated or the date of creation in the payers system of record, whichever comes last. Apps will use the meta.lastUpdated values to determine if the reference resources are as of the current date or date of service.</t>
+  </si>
+  <si>
+    <t>1.0.9</t>
   </si>
 </sst>
 </file>
@@ -1400,7 +1400,7 @@
         <v>131</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1942,7 +1942,7 @@
         <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1">
@@ -1958,7 +1958,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1990,7 +1990,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CapabilityStatement with Oral Profile
</commit_message>
<xml_diff>
--- a/input/fsh/scripts/carin-bb-server.xlsx
+++ b/input/fsh/scripts/carin-bb-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\FHIR\FSH\DaVinciIG_Dev\CARINBB\carin-bb\input\fsh\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cspears/dev/fhir/fsh/davinci/carin/STU2/carin-bb/input/fsh/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF7B8EC-D207-4EDE-816B-A3DE20720FA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D6F513-A1A3-914E-884A-975059B2E6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2025" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32960" yWindow="-3000" windowWidth="29040" windowHeight="17800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="191">
   <si>
     <t>Element</t>
   </si>
@@ -638,12 +638,6 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-Coverage</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit,http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit-Inpatient-Institutional,
-http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit-Outpatient-Institutional,
-http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit-Pharmacy,
-http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit-Professional-NonClinician</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit</t>
@@ -699,9 +693,6 @@
     <t>1.1.0</t>
   </si>
   <si>
-    <t>../../../output\us-core-comparisons/spec.internals</t>
-  </si>
-  <si>
     <t>1. See the [General Security Considerations](7_Authorization_Authentication_and_Registration.html) section for requirements and recommendations.
 1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` unauthorized response code.</t>
   </si>
@@ -709,13 +700,29 @@
     <t>This Section describes the expected capabilities of the C4BB Server actor which is responsible for providing responses to the queries submitted by the C4BB Requestors. 
 The EOB Resource is the focal Consumer-Directed Payer Data Exchange (CDPDE) Resource. Several Reference Resources are defined directly/indirectly from the EOB: Coverage, Patient, Organization (Payer ID), Practioner, and Organization (Facility).
 The Coverage Reference Resource SHALL be returned with data that was effective as of the date of service of the claim; for example, the data will reflect the employer name in effect at that time. However, for other reference resources, payers MAY decide to provide either the data that was in effect as of the date of service or the current data. All reference resources within the EOB will have meta.lastUpdated flagged as must support. Payers SHALL provide the last time the data was updated or the date of creation in the payers system of record, whichever comes last. Apps will use the meta.lastUpdated values to determine if the reference resources are as of the current date or date of service.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit-Oral</t>
+  </si>
+  <si>
+    <t>C4BB-ExplanationOfBenefit-Oral</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit,http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit-Inpatient-Institutional,
+http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit-Outpatient-Institutional,
+http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit-Oral,
+http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit-Pharmacy,
+http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-ExplanationOfBenefit-Professional-NonClinician</t>
+  </si>
+  <si>
+    <t>../../../output/us-core-comparisons/spec.internals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -944,7 +951,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -969,6 +975,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -1287,16 +1294,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C527BFB-CCF4-354D-B696-43330F2FE9C6}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="61.85546875" customWidth="1"/>
+    <col min="2" max="2" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1304,7 +1311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -1315,7 +1322,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
@@ -1323,7 +1330,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>113</v>
       </c>
@@ -1331,7 +1338,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>114</v>
       </c>
@@ -1339,7 +1346,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>115</v>
       </c>
@@ -1347,7 +1354,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>116</v>
       </c>
@@ -1355,7 +1362,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>122</v>
       </c>
@@ -1363,7 +1370,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>122</v>
       </c>
@@ -1371,7 +1378,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -1379,7 +1386,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -1387,7 +1394,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -1395,12 +1402,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>131</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1419,21 +1426,21 @@
       <selection activeCell="A2" sqref="A2:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="96.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="88.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="82.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="96.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="88.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="82.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -1465,386 +1472,386 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="81.95" customHeight="1" thickTop="1">
-      <c r="C2" s="30"/>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="82" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="29"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="C3" s="30"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C3" s="29"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10">
-      <c r="C4" s="30"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="29"/>
       <c r="E4"/>
       <c r="F4"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10">
-      <c r="C5" s="30"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C5" s="29"/>
       <c r="E5"/>
       <c r="F5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10">
-      <c r="C6" s="30"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C6" s="29"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10">
-      <c r="C7" s="30"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C7" s="29"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10">
-      <c r="C8" s="30"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C8" s="29"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10">
-      <c r="C9" s="30"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C9" s="29"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10">
-      <c r="C10" s="30"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="29"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="H10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10">
-      <c r="C11" s="30"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="29"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10">
-      <c r="C12" s="30"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="29"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="H12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1">
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1">
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="8:10">
+    <row r="17" spans="8:10" x14ac:dyDescent="0.2">
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="8:10" s="1" customFormat="1">
+    <row r="18" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="8:10" s="1" customFormat="1">
+    <row r="19" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="8:10" s="1" customFormat="1">
+    <row r="20" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="8:10">
+    <row r="21" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="8:10" s="1" customFormat="1">
+    <row r="22" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="8:10" s="1" customFormat="1">
+    <row r="23" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="8:10" s="1" customFormat="1">
+    <row r="24" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="8:10" s="1" customFormat="1">
+    <row r="25" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="8:10" s="1" customFormat="1">
+    <row r="26" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="8:10" s="1" customFormat="1">
+    <row r="27" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="8:10" s="1" customFormat="1">
+    <row r="28" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="8:10" s="1" customFormat="1">
+    <row r="29" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="8:10" s="1" customFormat="1">
+    <row r="30" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="8:10" s="1" customFormat="1">
+    <row r="31" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="8:10" s="1" customFormat="1">
+    <row r="32" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="3:10" s="1" customFormat="1">
+    <row r="33" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="3:10" s="1" customFormat="1">
+    <row r="34" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="3:10" s="1" customFormat="1">
+    <row r="35" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="3:10" s="1" customFormat="1">
+    <row r="36" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="3:10" s="1" customFormat="1">
+    <row r="37" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="3:10" s="1" customFormat="1">
+    <row r="38" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="3:10" s="1" customFormat="1">
+    <row r="39" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="40" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H40" s="5"/>
       <c r="I40" s="7"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="41" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H41" s="5"/>
       <c r="I41" s="7"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="42" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H42" s="5"/>
       <c r="I42" s="7"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="3:10" s="1" customFormat="1">
+    <row r="43" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="3:10" s="1" customFormat="1">
+    <row r="44" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C44" s="9"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="3:10" s="1" customFormat="1">
+    <row r="45" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C45" s="9"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="3:10" s="1" customFormat="1">
+    <row r="46" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C46" s="9"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="3:10" s="1" customFormat="1">
+    <row r="47" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C47" s="9"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="3:10" s="1" customFormat="1">
+    <row r="48" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C48" s="9"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="3:10" s="1" customFormat="1">
+    <row r="49" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="3:10" s="1" customFormat="1">
+    <row r="50" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="3:10" s="1" customFormat="1">
+    <row r="51" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="3:10" s="1" customFormat="1">
+    <row r="52" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="3:10" s="1" customFormat="1">
+    <row r="53" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="3:10" s="1" customFormat="1">
+    <row r="54" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="3:10" s="1" customFormat="1">
+    <row r="55" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="3:10" s="1" customFormat="1">
+    <row r="56" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="3:10" s="1" customFormat="1">
+    <row r="57" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="3:10" s="1" customFormat="1">
+    <row r="58" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="3:10" s="1" customFormat="1">
+    <row r="59" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="3:10" s="1" customFormat="1">
+    <row r="60" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="3:10" s="1" customFormat="1">
+    <row r="61" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="3:10" s="1" customFormat="1">
+    <row r="62" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="3:10" s="1" customFormat="1">
+    <row r="63" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C63" s="9"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="3:10" s="1" customFormat="1">
+    <row r="64" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C64" s="9"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="3:16" s="1" customFormat="1">
+    <row r="65" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="3:16" s="1" customFormat="1">
+    <row r="66" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C66" s="9"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="3:16" s="1" customFormat="1">
+    <row r="67" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C67" s="9"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="3:16" s="1" customFormat="1">
+    <row r="68" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C68" s="9"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="3:16" s="1" customFormat="1">
+    <row r="69" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C69" s="9"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="3:16" s="1" customFormat="1">
+    <row r="70" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" spans="3:16" s="1" customFormat="1" ht="15.75">
+    <row r="71" spans="3:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="C71" s="8"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="3:16" s="1" customFormat="1">
+    <row r="72" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="3:16" s="1" customFormat="1">
+    <row r="73" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="3:16" s="1" customFormat="1">
+    <row r="74" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="3:16" s="1" customFormat="1">
+    <row r="75" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="3:16">
+    <row r="76" spans="3:16" x14ac:dyDescent="0.2">
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
@@ -1855,37 +1862,37 @@
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
     </row>
-    <row r="77" spans="3:16" s="1" customFormat="1">
+    <row r="77" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+    <row r="78" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="3:16" s="1" customFormat="1">
+    <row r="79" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+    <row r="80" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H80" s="5"/>
       <c r="I80" s="7"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="8:10" s="1" customFormat="1">
+    <row r="81" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="8:10" s="1" customFormat="1" ht="20.25" customHeight="1">
+    <row r="82" spans="8:10" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
     </row>
-    <row r="83" spans="8:10" s="1" customFormat="1">
+    <row r="83" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
@@ -1903,17 +1910,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1921,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1929,23 +1936,23 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="15.75">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="1" customFormat="1">
+    </row>
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="1" customFormat="1">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>111</v>
       </c>
@@ -1953,15 +1960,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="257.10000000000002" customHeight="1">
+    <row r="6" spans="1:2" ht="257" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="34" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6" s="33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1969,7 +1976,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1977,20 +1984,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="351.75" customHeight="1">
+    <row r="9" spans="1:2" ht="351.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="103.5" customHeight="1">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2009,9 +2016,9 @@
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2026,65 +2033,65 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="105" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="114.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="114.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="27" customFormat="1" ht="23.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:6" s="26" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="18.75">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75">
-      <c r="A3" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="25" t="s">
+      <c r="C3" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>135</v>
       </c>
       <c r="E3" t="b">
@@ -2092,17 +2099,17 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
-      <c r="A4" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="25" t="s">
+    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="25" t="s">
+      <c r="C4" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>135</v>
       </c>
       <c r="E4" s="1" t="b">
@@ -2110,35 +2117,31 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="18.75">
-      <c r="A5" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="B5" s="25" t="s">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.75">
-      <c r="A6" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="25" t="s">
+      <c r="C6" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>135</v>
       </c>
       <c r="E6" s="1" t="b">
@@ -2146,84 +2149,98 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75">
-      <c r="A7" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>134</v>
+    <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>135</v>
       </c>
       <c r="E7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75">
-      <c r="A8" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>84</v>
+    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>134</v>
       </c>
       <c r="E8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="18.75">
-      <c r="A9" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>85</v>
+    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>84</v>
       </c>
       <c r="E9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="18.75">
-      <c r="A10" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>22</v>
+    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>85</v>
       </c>
       <c r="E10" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Outpatient-Facility" xr:uid="{DB5855A9-36F9-B146-BC04-BF373D3B96B6}"/>
-    <hyperlink ref="A2" r:id="rId2" display="http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit" xr:uid="{354343EB-05FC-BE4A-A5C5-AB9258320A2C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2232,28 +2249,28 @@
   <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="25.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
-    <col min="5" max="12" width="17.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.42578125" style="1" customWidth="1"/>
-    <col min="14" max="17" width="17.42578125" style="1" customWidth="1"/>
-    <col min="18" max="19" width="20.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="36.7109375" style="2" customWidth="1"/>
-    <col min="21" max="23" width="38.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="72.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="5" max="12" width="17.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" style="1" customWidth="1"/>
+    <col min="14" max="17" width="17.5" style="1" customWidth="1"/>
+    <col min="18" max="19" width="20.5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="36.6640625" style="2" customWidth="1"/>
+    <col min="21" max="23" width="38.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="72.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="25.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:24" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2327,7 +2344,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="19.5" thickTop="1">
+    <row r="2" spans="1:24" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>134</v>
       </c>
@@ -2342,22 +2359,22 @@
       <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="32" t="s">
+      <c r="T2" s="31" t="s">
         <v>155</v>
       </c>
       <c r="V2" s="20"/>
       <c r="W2" s="20"/>
       <c r="X2"/>
     </row>
-    <row r="3" spans="1:24" ht="315">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:24" ht="305" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>21</v>
@@ -2370,7 +2387,7 @@
       </c>
       <c r="W3" s="20"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
@@ -2386,7 +2403,7 @@
       <c r="V4" s="20"/>
       <c r="W4" s="20"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
@@ -2402,7 +2419,7 @@
       <c r="V5" s="20"/>
       <c r="W5" s="20"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2417,18 +2434,18 @@
       </c>
       <c r="W6" s="20"/>
     </row>
-    <row r="7" spans="1:24" ht="25.5" customHeight="1">
+    <row r="7" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:24" ht="25.5" customHeight="1">
+    <row r="8" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8"/>
     </row>
-    <row r="39" spans="20:23" ht="25.5" customHeight="1">
+    <row r="39" spans="20:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T39" s="21"/>
       <c r="V39" s="21"/>
       <c r="W39" s="21"/>
     </row>
-    <row r="42" spans="20:23" ht="25.5" customHeight="1">
+    <row r="42" spans="20:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="W42" s="21"/>
     </row>
   </sheetData>
@@ -2449,15 +2466,15 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2474,7 +2491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E2" s="2"/>
     </row>
   </sheetData>
@@ -2493,19 +2510,19 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
     <col min="2" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2534,7 +2551,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2543,7 +2560,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2555,7 +2572,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="180">
+    <row r="4" spans="1:9" ht="160" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2584,7 +2601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -2605,7 +2622,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -2614,7 +2631,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -2623,7 +2640,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -2632,7 +2649,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2641,7 +2658,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2650,7 +2667,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
       <c r="H12" s="1"/>
@@ -2669,13 +2686,13 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="51.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -2686,28 +2703,28 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="59.25" customHeight="1">
+    <row r="2" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>110</v>
       </c>
@@ -2724,44 +2741,44 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="J13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="43" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="75.42578125" style="31" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="75.5" style="30" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.5" customWidth="1"/>
+    <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="15" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" style="1" customWidth="1"/>
     <col min="20" max="20" width="15" style="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.83203125" style="1" customWidth="1"/>
     <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="38.28515625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="24.28515625" style="2" customWidth="1"/>
-    <col min="28" max="28" width="38.140625" customWidth="1"/>
+    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="38.33203125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="24.33203125" style="2" customWidth="1"/>
+    <col min="28" max="28" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18" thickBot="1">
+    <row r="1" spans="1:28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -2777,7 +2794,7 @@
       <c r="E1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>39</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -2847,7 +2864,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="13" customFormat="1" ht="15.75" thickTop="1">
+    <row r="2" spans="1:28" s="13" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2863,7 +2880,7 @@
       <c r="E2" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="29" t="str">
+      <c r="F2" s="28" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example category search</v>
       </c>
@@ -2894,7 +2911,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="13" customFormat="1" ht="15">
+    <row r="3" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -2910,7 +2927,7 @@
       <c r="E3" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="29" t="str">
+      <c r="F3" s="28" t="str">
         <f t="shared" ref="F3:F8" si="1">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B3)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example code search</v>
       </c>
@@ -2941,7 +2958,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="13" customFormat="1" ht="15">
+    <row r="4" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -2957,7 +2974,7 @@
       <c r="E4" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="29" t="str">
+      <c r="F4" s="28" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example date search</v>
       </c>
@@ -2989,7 +3006,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="13" customFormat="1" ht="72">
+    <row r="5" spans="1:28" s="13" customFormat="1" ht="61" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -3005,7 +3022,7 @@
       <c r="E5" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="29" t="str">
+      <c r="F5" s="28" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example patient search</v>
       </c>
@@ -3042,7 +3059,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="13" customFormat="1" ht="15">
+    <row r="6" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -3058,7 +3075,7 @@
       <c r="E6" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="29" t="str">
+      <c r="F6" s="28" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example status search</v>
       </c>
@@ -3089,7 +3106,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="13" customFormat="1" ht="15">
+    <row r="7" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -3105,7 +3122,7 @@
       <c r="E7" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="29" t="str">
+      <c r="F7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
@@ -3138,7 +3155,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="13" customFormat="1" ht="15">
+    <row r="8" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -3154,7 +3171,7 @@
       <c r="E8" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="29" t="str">
+      <c r="F8" s="28" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
@@ -3186,7 +3203,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="96">
+    <row r="9" spans="1:28" ht="78" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -3202,8 +3219,8 @@
       <c r="E9" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="30" t="s">
-        <v>172</v>
+      <c r="F9" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="G9" t="s">
         <v>57</v>
@@ -3233,7 +3250,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-_id.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="96">
+    <row r="10" spans="1:28" ht="78" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f>A9+1</f>
         <v>2</v>
@@ -3250,8 +3267,8 @@
       <c r="E10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="30" t="s">
-        <v>172</v>
+      <c r="F10" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="G10" t="s">
         <v>57</v>
@@ -3287,7 +3304,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="96">
+    <row r="11" spans="1:28" ht="78" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" ref="A11:A19" si="9">A10+1</f>
         <v>3</v>
@@ -3304,8 +3321,8 @@
       <c r="E11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="30" t="s">
-        <v>172</v>
+      <c r="F11" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="G11" t="s">
         <v>57</v>
@@ -3339,7 +3356,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-_lastupdated.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="96">
+    <row r="12" spans="1:28" ht="78" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="9"/>
         <v>4</v>
@@ -3356,8 +3373,8 @@
       <c r="E12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F12" s="30" t="s">
-        <v>172</v>
+      <c r="F12" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="G12" t="s">
         <v>57</v>
@@ -3388,7 +3405,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-type.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="13" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="9"/>
         <v>5</v>
@@ -3405,8 +3422,8 @@
       <c r="E13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="30" t="s">
-        <v>172</v>
+      <c r="F13" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>57</v>
@@ -3437,7 +3454,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-identifier.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="96">
+    <row r="14" spans="1:28" ht="78" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="9"/>
         <v>6</v>
@@ -3454,8 +3471,8 @@
       <c r="E14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F14" s="30" t="s">
-        <v>172</v>
+      <c r="F14" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="G14" t="s">
         <v>57</v>
@@ -3486,7 +3503,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-service-date.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="9"/>
         <v>7</v>
@@ -3503,8 +3520,8 @@
       <c r="E15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="30" t="s">
-        <v>172</v>
+      <c r="F15" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>57</v>
@@ -3542,7 +3559,7 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-provider.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="16" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" si="9"/>
         <v>8</v>
@@ -3559,8 +3576,8 @@
       <c r="E16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="30" t="s">
-        <v>172</v>
+      <c r="F16" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>57</v>
@@ -3598,7 +3615,7 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-care-team.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="17" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" si="9"/>
         <v>9</v>
@@ -3615,8 +3632,8 @@
       <c r="E17" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F17" s="30" t="s">
-        <v>172</v>
+      <c r="F17" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>57</v>
@@ -3654,7 +3671,7 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-insurer.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="18" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" si="9"/>
         <v>10</v>
@@ -3671,8 +3688,8 @@
       <c r="E18" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F18" s="30" t="s">
-        <v>172</v>
+      <c r="F18" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
@@ -3710,7 +3727,7 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-facility.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="19" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="9"/>
         <v>11</v>
@@ -3727,8 +3744,8 @@
       <c r="E19" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F19" s="30" t="s">
-        <v>172</v>
+      <c r="F19" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>57</v>
@@ -3766,7 +3783,7 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-coverage.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="18.95" customHeight="1">
+    <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f>A19+1</f>
         <v>12</v>
@@ -3783,7 +3800,7 @@
       <c r="E20" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="34" t="s">
         <v>171</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -3814,68 +3831,68 @@
         <v>SearchParameter-carin-bb-!coverage-_id.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
-      <c r="F21" s="31"/>
+    <row r="21" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="30"/>
       <c r="Y21" s="17"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="18.95" customHeight="1">
+    <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="Y22" s="17"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" ht="18.95" customHeight="1">
+    <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="Y23" s="17"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="18.95" customHeight="1">
+    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="Y24" s="17"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="18.95" customHeight="1">
+    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="Y25" s="17"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" ht="18.95" customHeight="1">
+    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="Y26" s="17"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" ht="18.95" customHeight="1">
+    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="Y27" s="17"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" ht="18.95" customHeight="1">
+    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="Y28" s="17"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" ht="18.95" customHeight="1">
+    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="Y29" s="17"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" ht="18.95" customHeight="1">
+    <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -3887,11 +3904,8 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA19">
     <sortCondition ref="B1"/>
   </sortState>
-  <hyperlinks>
-    <hyperlink ref="F20" r:id="rId1" display="http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-Coverage" xr:uid="{A7BD924E-2AE3-E944-BA4C-5FB895D21DE3}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to publish as 1.1.0
</commit_message>
<xml_diff>
--- a/input/fsh/scripts/carin-bb-server.xlsx
+++ b/input/fsh/scripts/carin-bb-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\FHIR\FSH\DaVinciIG_Dev\CARINBB\carin-bb\input\fsh\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cspears/dev/fhir/fsh/davinci/carin/carin-bb/input/fsh/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF7B8EC-D207-4EDE-816B-A3DE20720FA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE6CECE-E649-4D4A-91FE-DF7BAF35FE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2025" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29040" yWindow="-2780" windowWidth="29040" windowHeight="17800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -699,9 +699,6 @@
     <t>1.1.0</t>
   </si>
   <si>
-    <t>../../../output\us-core-comparisons/spec.internals</t>
-  </si>
-  <si>
     <t>1. See the [General Security Considerations](7_Authorization_Authentication_and_Registration.html) section for requirements and recommendations.
 1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` unauthorized response code.</t>
   </si>
@@ -709,13 +706,16 @@
     <t>This Section describes the expected capabilities of the C4BB Server actor which is responsible for providing responses to the queries submitted by the C4BB Requestors. 
 The EOB Resource is the focal Consumer-Directed Payer Data Exchange (CDPDE) Resource. Several Reference Resources are defined directly/indirectly from the EOB: Coverage, Patient, Organization (Payer ID), Practioner, and Organization (Facility).
 The Coverage Reference Resource SHALL be returned with data that was effective as of the date of service of the claim; for example, the data will reflect the employer name in effect at that time. However, for other reference resources, payers MAY decide to provide either the data that was in effect as of the date of service or the current data. All reference resources within the EOB will have meta.lastUpdated flagged as must support. Payers SHALL provide the last time the data was updated or the date of creation in the payers system of record, whichever comes last. Apps will use the meta.lastUpdated values to determine if the reference resources are as of the current date or date of service.</t>
+  </si>
+  <si>
+    <t>../../../output/us-core-comparisons/spec.internals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1287,16 +1287,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C527BFB-CCF4-354D-B696-43330F2FE9C6}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="61.85546875" customWidth="1"/>
+    <col min="2" max="2" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>113</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>114</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>115</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>116</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>122</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>122</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -1395,12 +1395,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>131</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1419,21 +1419,21 @@
       <selection activeCell="A2" sqref="A2:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="96.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="88.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="82.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="96.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="88.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="82.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -1465,50 +1465,50 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="81.95" customHeight="1" thickTop="1">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="82" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C2" s="30"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C3" s="30"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="30"/>
       <c r="E4"/>
       <c r="F4"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="30"/>
       <c r="E5"/>
       <c r="F5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="30"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="30"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C8" s="30"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9" s="30"/>
       <c r="E9"/>
       <c r="F9"/>
@@ -1516,335 +1516,335 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" s="30"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="H10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C11" s="30"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" s="30"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="H12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1">
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1">
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="8:10">
+    <row r="17" spans="8:10" x14ac:dyDescent="0.2">
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="8:10" s="1" customFormat="1">
+    <row r="18" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="8:10" s="1" customFormat="1">
+    <row r="19" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="8:10" s="1" customFormat="1">
+    <row r="20" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="8:10">
+    <row r="21" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="8:10" s="1" customFormat="1">
+    <row r="22" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="8:10" s="1" customFormat="1">
+    <row r="23" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="8:10" s="1" customFormat="1">
+    <row r="24" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="8:10" s="1" customFormat="1">
+    <row r="25" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="8:10" s="1" customFormat="1">
+    <row r="26" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="8:10" s="1" customFormat="1">
+    <row r="27" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="8:10" s="1" customFormat="1">
+    <row r="28" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="8:10" s="1" customFormat="1">
+    <row r="29" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="8:10" s="1" customFormat="1">
+    <row r="30" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="8:10" s="1" customFormat="1">
+    <row r="31" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="8:10" s="1" customFormat="1">
+    <row r="32" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="3:10" s="1" customFormat="1">
+    <row r="33" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="3:10" s="1" customFormat="1">
+    <row r="34" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="3:10" s="1" customFormat="1">
+    <row r="35" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="3:10" s="1" customFormat="1">
+    <row r="36" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="3:10" s="1" customFormat="1">
+    <row r="37" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="3:10" s="1" customFormat="1">
+    <row r="38" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="3:10" s="1" customFormat="1">
+    <row r="39" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="40" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H40" s="5"/>
       <c r="I40" s="7"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="41" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H41" s="5"/>
       <c r="I41" s="7"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="42" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H42" s="5"/>
       <c r="I42" s="7"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="3:10" s="1" customFormat="1">
+    <row r="43" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="3:10" s="1" customFormat="1">
+    <row r="44" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C44" s="9"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="3:10" s="1" customFormat="1">
+    <row r="45" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C45" s="9"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="3:10" s="1" customFormat="1">
+    <row r="46" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C46" s="9"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="3:10" s="1" customFormat="1">
+    <row r="47" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C47" s="9"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="3:10" s="1" customFormat="1">
+    <row r="48" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C48" s="9"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="3:10" s="1" customFormat="1">
+    <row r="49" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="3:10" s="1" customFormat="1">
+    <row r="50" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="3:10" s="1" customFormat="1">
+    <row r="51" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="3:10" s="1" customFormat="1">
+    <row r="52" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="3:10" s="1" customFormat="1">
+    <row r="53" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="3:10" s="1" customFormat="1">
+    <row r="54" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="3:10" s="1" customFormat="1">
+    <row r="55" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="3:10" s="1" customFormat="1">
+    <row r="56" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="3:10" s="1" customFormat="1">
+    <row r="57" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="3:10" s="1" customFormat="1">
+    <row r="58" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="3:10" s="1" customFormat="1">
+    <row r="59" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="3:10" s="1" customFormat="1">
+    <row r="60" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="3:10" s="1" customFormat="1">
+    <row r="61" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="3:10" s="1" customFormat="1">
+    <row r="62" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="3:10" s="1" customFormat="1">
+    <row r="63" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C63" s="9"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="3:10" s="1" customFormat="1">
+    <row r="64" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C64" s="9"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="3:16" s="1" customFormat="1">
+    <row r="65" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="3:16" s="1" customFormat="1">
+    <row r="66" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C66" s="9"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="3:16" s="1" customFormat="1">
+    <row r="67" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C67" s="9"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="3:16" s="1" customFormat="1">
+    <row r="68" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C68" s="9"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="3:16" s="1" customFormat="1">
+    <row r="69" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C69" s="9"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="3:16" s="1" customFormat="1">
+    <row r="70" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" spans="3:16" s="1" customFormat="1" ht="15.75">
+    <row r="71" spans="3:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="C71" s="8"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="3:16" s="1" customFormat="1">
+    <row r="72" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="3:16" s="1" customFormat="1">
+    <row r="73" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="3:16" s="1" customFormat="1">
+    <row r="74" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="3:16" s="1" customFormat="1">
+    <row r="75" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="3:16">
+    <row r="76" spans="3:16" x14ac:dyDescent="0.2">
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
@@ -1855,37 +1855,37 @@
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
     </row>
-    <row r="77" spans="3:16" s="1" customFormat="1">
+    <row r="77" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+    <row r="78" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="3:16" s="1" customFormat="1">
+    <row r="79" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+    <row r="80" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H80" s="5"/>
       <c r="I80" s="7"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="8:10" s="1" customFormat="1">
+    <row r="81" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="8:10" s="1" customFormat="1" ht="20.25" customHeight="1">
+    <row r="82" spans="8:10" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
     </row>
-    <row r="83" spans="8:10" s="1" customFormat="1">
+    <row r="83" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
@@ -1903,17 +1903,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="15.75">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>181</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1">
+    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>111</v>
       </c>
@@ -1953,15 +1953,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="257.10000000000002" customHeight="1">
+    <row r="6" spans="1:2" ht="257" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="351.75" customHeight="1">
+    <row r="9" spans="1:2" ht="351.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1985,12 +1985,12 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="103.5" customHeight="1">
+    <row r="10" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2009,9 +2009,9 @@
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2032,15 +2032,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="114.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="114.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="27" customFormat="1" ht="23.25">
+    <row r="1" spans="1:6" s="27" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="18.75">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>173</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
+    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>174</v>
       </c>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
+    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>175</v>
       </c>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="18.75">
+    <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>176</v>
       </c>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75">
+    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>177</v>
       </c>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75">
+    <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>171</v>
       </c>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75">
+    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>178</v>
       </c>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="18.75">
+    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>179</v>
       </c>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="18.75">
+    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>180</v>
       </c>
@@ -2238,22 +2238,22 @@
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="25.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
-    <col min="5" max="12" width="17.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.42578125" style="1" customWidth="1"/>
-    <col min="14" max="17" width="17.42578125" style="1" customWidth="1"/>
-    <col min="18" max="19" width="20.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="36.7109375" style="2" customWidth="1"/>
-    <col min="21" max="23" width="38.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="72.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="5" max="12" width="17.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" style="1" customWidth="1"/>
+    <col min="14" max="17" width="17.5" style="1" customWidth="1"/>
+    <col min="18" max="19" width="20.5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="36.6640625" style="2" customWidth="1"/>
+    <col min="21" max="23" width="38.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="72.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="25.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:24" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="19.5" thickTop="1">
+    <row r="2" spans="1:24" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>134</v>
       </c>
@@ -2349,7 +2349,7 @@
       <c r="W2" s="20"/>
       <c r="X2"/>
     </row>
-    <row r="3" spans="1:24" ht="315">
+    <row r="3" spans="1:24" ht="305" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>135</v>
       </c>
@@ -2370,7 +2370,7 @@
       </c>
       <c r="W3" s="20"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
@@ -2386,7 +2386,7 @@
       <c r="V4" s="20"/>
       <c r="W4" s="20"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="V5" s="20"/>
       <c r="W5" s="20"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2417,18 +2417,18 @@
       </c>
       <c r="W6" s="20"/>
     </row>
-    <row r="7" spans="1:24" ht="25.5" customHeight="1">
+    <row r="7" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:24" ht="25.5" customHeight="1">
+    <row r="8" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8"/>
     </row>
-    <row r="39" spans="20:23" ht="25.5" customHeight="1">
+    <row r="39" spans="20:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T39" s="21"/>
       <c r="V39" s="21"/>
       <c r="W39" s="21"/>
     </row>
-    <row r="42" spans="20:23" ht="25.5" customHeight="1">
+    <row r="42" spans="20:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="W42" s="21"/>
     </row>
   </sheetData>
@@ -2449,15 +2449,15 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E2" s="2"/>
     </row>
   </sheetData>
@@ -2493,19 +2493,19 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
     <col min="2" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2543,7 +2543,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2555,7 +2555,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="180">
+    <row r="4" spans="1:9" ht="160" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -2614,7 +2614,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -2623,7 +2623,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -2632,7 +2632,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2641,7 +2641,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2650,7 +2650,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
       <c r="H12" s="1"/>
@@ -2669,13 +2669,13 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="51.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -2686,28 +2686,28 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="59.25" customHeight="1">
+    <row r="2" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>110</v>
       </c>
@@ -2730,38 +2730,38 @@
       <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="43" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="75.42578125" style="31" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="75.5" style="31" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.5" customWidth="1"/>
+    <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="15" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" style="1" customWidth="1"/>
     <col min="20" max="20" width="15" style="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.83203125" style="1" customWidth="1"/>
     <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="38.28515625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="24.28515625" style="2" customWidth="1"/>
-    <col min="28" max="28" width="38.140625" customWidth="1"/>
+    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="38.33203125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="24.33203125" style="2" customWidth="1"/>
+    <col min="28" max="28" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18" thickBot="1">
+    <row r="1" spans="1:28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="13" customFormat="1" ht="15.75" thickTop="1">
+    <row r="2" spans="1:28" s="13" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="13" customFormat="1" ht="15">
+    <row r="3" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="13" customFormat="1" ht="15">
+    <row r="4" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="13" customFormat="1" ht="72">
+    <row r="5" spans="1:28" s="13" customFormat="1" ht="61" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="13" customFormat="1" ht="15">
+    <row r="6" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="13" customFormat="1" ht="15">
+    <row r="7" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="13" customFormat="1" ht="15">
+    <row r="8" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="96">
+    <row r="9" spans="1:28" ht="65" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-_id.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="96">
+    <row r="10" spans="1:28" ht="65" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f>A9+1</f>
         <v>2</v>
@@ -3287,7 +3287,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="96">
+    <row r="11" spans="1:28" ht="65" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" ref="A11:A19" si="9">A10+1</f>
         <v>3</v>
@@ -3339,7 +3339,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-_lastupdated.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="96">
+    <row r="12" spans="1:28" ht="65" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="9"/>
         <v>4</v>
@@ -3388,7 +3388,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-type.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="13" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="9"/>
         <v>5</v>
@@ -3437,7 +3437,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-identifier.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="96">
+    <row r="14" spans="1:28" ht="65" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="9"/>
         <v>6</v>
@@ -3486,7 +3486,7 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-service-date.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="9"/>
         <v>7</v>
@@ -3542,7 +3542,7 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-provider.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="16" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" si="9"/>
         <v>8</v>
@@ -3598,7 +3598,7 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-care-team.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="17" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" si="9"/>
         <v>9</v>
@@ -3654,7 +3654,7 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-insurer.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="18" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" si="9"/>
         <v>10</v>
@@ -3710,7 +3710,7 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-facility.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" s="1" customFormat="1" ht="96">
+    <row r="19" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="9"/>
         <v>11</v>
@@ -3766,7 +3766,7 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-coverage.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="18.95" customHeight="1">
+    <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f>A19+1</f>
         <v>12</v>
@@ -3814,68 +3814,68 @@
         <v>SearchParameter-carin-bb-!coverage-_id.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="21" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F21" s="31"/>
       <c r="Y21" s="17"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="18.95" customHeight="1">
+    <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="Y22" s="17"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" ht="18.95" customHeight="1">
+    <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="Y23" s="17"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="18.95" customHeight="1">
+    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="Y24" s="17"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="18.95" customHeight="1">
+    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="Y25" s="17"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" ht="18.95" customHeight="1">
+    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="Y26" s="17"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" ht="18.95" customHeight="1">
+    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="Y27" s="17"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" ht="18.95" customHeight="1">
+    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="Y28" s="17"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" ht="18.95" customHeight="1">
+    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="Y29" s="17"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" ht="18.95" customHeight="1">
+    <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>

</xml_diff>

<commit_message>
add RelatedPerson to xlsx file...can't yet regenerate CapStmt due to tooling issue
</commit_message>
<xml_diff>
--- a/input/fsh/scripts/carin-bb-server.xlsx
+++ b/input/fsh/scripts/carin-bb-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cspears/dev/fhir/fsh/davinci/carin/carin-bb/input/fsh/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/carin-bb/input/fsh/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901209AD-0CF9-1E45-AC0B-F8A4F62DFACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8023B32-A994-964B-BF19-C99A8F390FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37260" yWindow="-1960" windowWidth="46480" windowHeight="27060" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="2900" windowWidth="46160" windowHeight="20500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="195">
   <si>
     <t>Element</t>
   </si>
@@ -679,9 +679,6 @@
 </t>
   </si>
   <si>
-    <t>1.1.0</t>
-  </si>
-  <si>
     <t>1. See the [General Security Considerations](7_Authorization_Authentication_and_Registration.html) section for requirements and recommendations.
 1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` unauthorized response code.</t>
   </si>
@@ -721,12 +718,24 @@
   <si>
     <t>billable-period-start</t>
   </si>
+  <si>
+    <t>2.0.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/C4BB-RelatedPerson</t>
+  </si>
+  <si>
+    <t>C4BB-RelatedPerson</t>
+  </si>
+  <si>
+    <t>RelatedPerson</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -853,13 +862,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="1"/>
@@ -956,10 +958,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -972,7 +973,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -980,6 +981,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -1411,7 +1413,7 @@
         <v>131</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1477,50 +1479,50 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="82" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="29"/>
+      <c r="C2" s="28"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C3" s="29"/>
+      <c r="C3" s="28"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="29"/>
+      <c r="C4" s="28"/>
       <c r="E4"/>
       <c r="F4"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C5" s="29"/>
+      <c r="C5" s="28"/>
       <c r="E5"/>
       <c r="F5"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C6" s="29"/>
+      <c r="C6" s="28"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="29"/>
+      <c r="C7" s="28"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="29"/>
+      <c r="C8" s="28"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="29"/>
+      <c r="C9" s="28"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="H9" s="5"/>
@@ -1528,20 +1530,20 @@
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C10" s="29"/>
+      <c r="C10" s="28"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="H10" s="5"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C11" s="29"/>
+      <c r="C11" s="28"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="29"/>
+      <c r="C12" s="28"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="H12" s="5"/>
@@ -1914,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1953,7 +1955,7 @@
         <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1968,8 +1970,8 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>183</v>
+      <c r="B6" s="32" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2001,7 +2003,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2037,10 +2039,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="105" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2051,20 +2053,20 @@
     <col min="4" max="4" width="31.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="26" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:6" s="25" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2072,16 +2074,16 @@
       <c r="A2" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="24" t="s">
+      <c r="C2" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="23" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2089,13 +2091,13 @@
       <c r="A3" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>135</v>
       </c>
       <c r="E3" t="b">
@@ -2107,13 +2109,13 @@
       <c r="A4" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>135</v>
       </c>
       <c r="E4" s="1" t="b">
@@ -2123,15 +2125,15 @@
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="24" t="s">
+      <c r="C5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>135</v>
       </c>
       <c r="E5" s="1" t="b">
@@ -2142,13 +2144,13 @@
       <c r="A6" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="C6" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>135</v>
       </c>
       <c r="E6" s="1" t="b">
@@ -2160,13 +2162,13 @@
       <c r="A7" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="24" t="s">
+      <c r="C7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>135</v>
       </c>
       <c r="E7" s="1" t="b">
@@ -2178,13 +2180,13 @@
       <c r="A8" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>134</v>
       </c>
       <c r="E8" s="1" t="b">
@@ -2196,13 +2198,13 @@
       <c r="A9" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="C9" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="24" t="s">
+      <c r="C9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>84</v>
       </c>
       <c r="E9" s="1" t="b">
@@ -2214,13 +2216,13 @@
       <c r="A10" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="24" t="s">
+      <c r="C10" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>85</v>
       </c>
       <c r="E10" s="1" t="b">
@@ -2229,25 +2231,46 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="1" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1" xr:uid="{9B794999-77AF-994F-94B5-734419EC7E92}"/>
+    <hyperlink ref="A11" r:id="rId2" xr:uid="{C9599929-5104-7841-AF03-EBA223AB5D12}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2255,11 +2278,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomRight" activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2366,7 +2389,7 @@
       <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="T2" s="30" t="s">
         <v>154</v>
       </c>
       <c r="V2" s="20"/>
@@ -2374,14 +2397,14 @@
       <c r="X2"/>
     </row>
     <row r="3" spans="1:24" ht="305" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>135</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>21</v>
@@ -2442,7 +2465,18 @@
       <c r="W6" s="20"/>
     </row>
     <row r="7" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7"/>
+      <c r="A7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8"/>
@@ -2576,7 +2610,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -2761,7 +2795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2775,7 +2809,7 @@
     <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="75.5" style="30" customWidth="1"/>
+    <col min="6" max="6" width="75.5" style="29" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" customWidth="1"/>
     <col min="9" max="9" width="23.5" customWidth="1"/>
     <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -2815,7 +2849,7 @@
       <c r="E1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>39</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -2901,7 +2935,7 @@
       <c r="E2" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="28" t="str">
+      <c r="F2" s="27" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example category search</v>
       </c>
@@ -2948,7 +2982,7 @@
       <c r="E3" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="28" t="str">
+      <c r="F3" s="27" t="str">
         <f t="shared" ref="F3:F8" si="1">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B3)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example code search</v>
       </c>
@@ -2995,7 +3029,7 @@
       <c r="E4" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="28" t="str">
+      <c r="F4" s="27" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example date search</v>
       </c>
@@ -3043,7 +3077,7 @@
       <c r="E5" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="28" t="str">
+      <c r="F5" s="27" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example patient search</v>
       </c>
@@ -3096,7 +3130,7 @@
       <c r="E6" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="28" t="str">
+      <c r="F6" s="27" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example status search</v>
       </c>
@@ -3143,7 +3177,7 @@
       <c r="E7" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="28" t="str">
+      <c r="F7" s="27" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
@@ -3192,7 +3226,7 @@
       <c r="E8" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="28" t="str">
+      <c r="F8" s="27" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
@@ -3240,8 +3274,8 @@
       <c r="E9" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="29" t="s">
-        <v>186</v>
+      <c r="F9" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G9" t="s">
         <v>57</v>
@@ -3294,8 +3328,8 @@
       <c r="E10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="29" t="s">
-        <v>186</v>
+      <c r="F10" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G10" t="s">
         <v>57</v>
@@ -3354,8 +3388,8 @@
       <c r="E11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="29" t="s">
-        <v>186</v>
+      <c r="F11" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G11" t="s">
         <v>57</v>
@@ -3412,8 +3446,8 @@
       <c r="E12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F12" s="29" t="s">
-        <v>186</v>
+      <c r="F12" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G12" t="s">
         <v>57</v>
@@ -3467,8 +3501,8 @@
       <c r="E13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="29" t="s">
-        <v>186</v>
+      <c r="F13" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>57</v>
@@ -3522,8 +3556,8 @@
       <c r="E14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F14" s="29" t="s">
-        <v>186</v>
+      <c r="F14" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G14" t="s">
         <v>57</v>
@@ -3569,7 +3603,7 @@
         <v>135</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -3577,8 +3611,8 @@
       <c r="E15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="29" t="s">
-        <v>186</v>
+      <c r="F15" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>57</v>
@@ -3625,7 +3659,7 @@
         <v>135</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -3633,8 +3667,8 @@
       <c r="E16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="29" t="s">
-        <v>186</v>
+      <c r="F16" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>57</v>
@@ -3689,8 +3723,8 @@
       <c r="E17" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F17" s="29" t="s">
-        <v>186</v>
+      <c r="F17" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>57</v>
@@ -3745,8 +3779,8 @@
       <c r="E18" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F18" s="29" t="s">
-        <v>186</v>
+      <c r="F18" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
@@ -3801,8 +3835,8 @@
       <c r="E19" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F19" s="29" t="s">
-        <v>186</v>
+      <c r="F19" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>57</v>
@@ -3857,8 +3891,8 @@
       <c r="E20" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="29" t="s">
-        <v>186</v>
+      <c r="F20" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>57</v>
@@ -3913,8 +3947,8 @@
       <c r="E21" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F21" s="29" t="s">
-        <v>186</v>
+      <c r="F21" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>57</v>
@@ -3969,7 +4003,7 @@
       <c r="E22" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F22" s="34" t="s">
+      <c r="F22" s="33" t="s">
         <v>169</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -4001,7 +4035,7 @@
       </c>
     </row>
     <row r="23" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F23" s="30"/>
+      <c r="F23" s="29"/>
       <c r="Y23" s="17"/>
       <c r="AA23" s="2"/>
     </row>

</xml_diff>

<commit_message>
FHIR-36676 - update lastUpdated to 0..1 MS, updated comment, and updated CapSTmt spreadsheet
</commit_message>
<xml_diff>
--- a/input/fsh/scripts/carin-bb-server.xlsx
+++ b/input/fsh/scripts/carin-bb-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/carin-bb/input/fsh/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8023B32-A994-964B-BF19-C99A8F390FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7E0BA9-B0BC-8D4B-B37E-682A52F6A868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="2900" windowWidth="46160" windowHeight="20500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2042,7 +2042,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="105" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2202,7 +2202,7 @@
         <v>164</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>84</v>
@@ -2220,7 +2220,7 @@
         <v>165</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>85</v>
@@ -2279,10 +2279,10 @@
   <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y7" sqref="Y7"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2422,7 +2422,7 @@
         <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>21</v>
@@ -2438,7 +2438,7 @@
         <v>84</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
CapabilityStatement improvements and pre-apply of FHIR-38108
</commit_message>
<xml_diff>
--- a/input/fsh/scripts/carin-bb-server.xlsx
+++ b/input/fsh/scripts/carin-bb-server.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/carin-bb/input/fsh/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cspears/dev/fhir/fsh/davinci/carin/carin-bb/input/fsh/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7E0BA9-B0BC-8D4B-B37E-682A52F6A868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1208D910-C70F-3947-ACDE-20625D91DC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="2900" windowWidth="46160" windowHeight="20500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98520" yWindow="6320" windowWidth="51200" windowHeight="28300" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="196">
   <si>
     <t>Element</t>
   </si>
@@ -597,9 +597,6 @@
   </si>
   <si>
     <t>Abstract Profile, should go in profiles, not supporting_profiles</t>
-  </si>
-  <si>
-    <t>ExplanationOfBenefit:patient,ExplanationOfBenefit:provider,ExplanationOfBenefit:care-team,ExplanationOfBenefit:coverage,ExplanationOfBenefit:insurer,ExplanationOfBenefit:*</t>
   </si>
   <si>
     <t>C4BB-ExplanationOfBenefit</t>
@@ -729,6 +726,12 @@
   </si>
   <si>
     <t>RelatedPerson</t>
+  </si>
+  <si>
+    <t>conf_RelatedPerson</t>
+  </si>
+  <si>
+    <t>ExplanationOfBenefit:patient,ExplanationOfBenefit:provider,ExplanationOfBenefit:care-team,ExplanationOfBenefit:coverage,ExplanationOfBenefit:insurer,ExplanationOfBenefit:payee,ExplanationOfBenefit:*</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1416,7 @@
         <v>131</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1917,7 +1920,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1944,10 +1947,10 @@
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1955,7 +1958,7 @@
         <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1971,7 +1974,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1995,7 +1998,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2003,7 +2006,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2072,10 +2075,10 @@
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>13</v>
@@ -2089,10 +2092,10 @@
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>13</v>
@@ -2107,10 +2110,10 @@
     </row>
     <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>13</v>
@@ -2125,10 +2128,10 @@
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>183</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>184</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>13</v>
@@ -2142,10 +2145,10 @@
     </row>
     <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>13</v>
@@ -2160,10 +2163,10 @@
     </row>
     <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>13</v>
@@ -2178,10 +2181,10 @@
     </row>
     <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>13</v>
@@ -2196,10 +2199,10 @@
     </row>
     <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>63</v>
@@ -2214,10 +2217,10 @@
     </row>
     <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>63</v>
@@ -2232,10 +2235,10 @@
     </row>
     <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C11" s="23" t="s">
         <v>13</v>
@@ -2249,16 +2252,16 @@
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="23" t="s">
         <v>192</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>193</v>
       </c>
       <c r="C12" s="23" t="s">
         <v>63</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E12" s="1" t="b">
         <v>1</v>
@@ -2278,11 +2281,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4:B5"/>
+      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2404,7 +2407,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>21</v>
@@ -2413,7 +2416,7 @@
         <v>13</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="W3" s="20"/>
     </row>
@@ -2466,7 +2469,7 @@
     </row>
     <row r="7" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>63</v>
@@ -2542,13 +2545,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2562,9 +2565,10 @@
     <col min="7" max="7" width="81.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2592,8 +2596,11 @@
       <c r="I1" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2602,7 +2609,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="380" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="380" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2610,7 +2617,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -2627,8 +2634,11 @@
       <c r="I3" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2653,29 +2663,37 @@
       <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>63</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="H5" s="1" t="s">
         <v>63</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -2684,7 +2702,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -2693,7 +2711,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -2702,7 +2720,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2711,7 +2729,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2720,7 +2738,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
       <c r="H12" s="1"/>
@@ -2795,11 +2813,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="O12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S9" sqref="S9:S16"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3275,7 +3293,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G9" t="s">
         <v>57</v>
@@ -3287,8 +3305,8 @@
         <v>58</v>
       </c>
       <c r="J9" t="str">
-        <f>B9&amp;"."&amp;"managingOrganization"</f>
-        <v>ExplanationOfBenefit.managingOrganization</v>
+        <f>B9&amp;"."&amp;"id"</f>
+        <v>ExplanationOfBenefit.id</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>57</v>
@@ -3329,7 +3347,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G10" t="s">
         <v>57</v>
@@ -3389,7 +3407,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G11" t="s">
         <v>57</v>
@@ -3447,7 +3465,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G12" t="s">
         <v>57</v>
@@ -3502,7 +3520,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>57</v>
@@ -3557,7 +3575,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G14" t="s">
         <v>57</v>
@@ -3603,7 +3621,7 @@
         <v>135</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -3612,7 +3630,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>57</v>
@@ -3659,7 +3677,7 @@
         <v>135</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -3668,7 +3686,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>57</v>
@@ -3724,7 +3742,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>57</v>
@@ -3780,7 +3798,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
@@ -3836,7 +3854,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>57</v>
@@ -3892,7 +3910,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>57</v>
@@ -3948,7 +3966,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>57</v>
@@ -3960,7 +3978,7 @@
         <v>69</v>
       </c>
       <c r="J21" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f>B21&amp;"."&amp;C21</f>
         <v>!ExplanationOfBenefit.coverage</v>
       </c>
       <c r="K21" s="1" t="s">
@@ -4004,7 +4022,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>57</v>
@@ -4016,8 +4034,8 @@
         <v>58</v>
       </c>
       <c r="J22" s="1" t="str">
-        <f>B22&amp;"."&amp;"managingOrganization"</f>
-        <v>Coverage.managingOrganization</v>
+        <f>B22&amp;"."&amp;"id"</f>
+        <v>Coverage.id</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>57</v>
@@ -4026,6 +4044,9 @@
         <v>57</v>
       </c>
       <c r="S22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="Y22" s="17"/>
@@ -4035,30 +4056,205 @@
       </c>
     </row>
     <row r="23" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F23" s="29"/>
+      <c r="A23" s="1">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="1" t="str">
+        <f>B23&amp;"."&amp;"id"</f>
+        <v>Patient.id</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="Y23" s="17"/>
       <c r="AA23" s="2"/>
+      <c r="AB23" s="1" t="str">
+        <f>"SearchParameter-carin-bb-"&amp;LOWER((B23)&amp;"-"&amp;C23&amp;".html")</f>
+        <v>SearchParameter-carin-bb-patient-_id.html</v>
+      </c>
     </row>
     <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="A24" s="1">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="1" t="str">
+        <f t="shared" ref="J24:J26" si="18">B24&amp;"."&amp;"id"</f>
+        <v>Organization.id</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="Y24" s="17"/>
-      <c r="AB24" s="1"/>
+      <c r="AB24" s="1" t="str">
+        <f t="shared" ref="AB24:AB26" si="19">"SearchParameter-carin-bb-"&amp;LOWER((B24)&amp;"-"&amp;C24&amp;".html")</f>
+        <v>SearchParameter-carin-bb-organization-_id.html</v>
+      </c>
     </row>
     <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="A25" s="1">
+        <v>15</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>Practitioner.id</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="Y25" s="17"/>
-      <c r="AB25" s="1"/>
+      <c r="AB25" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>SearchParameter-carin-bb-practitioner-_id.html</v>
+      </c>
     </row>
     <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="A26" s="1">
+        <v>16</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J26" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>RelatedPerson.id</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="Y26" s="17"/>
-      <c r="AB26" s="1"/>
+      <c r="AB26" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>SearchParameter-carin-bb-relatedperson-_id.html</v>
+      </c>
     </row>
     <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G27" s="1"/>
@@ -4107,8 +4303,14 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA21">
     <sortCondition ref="B1"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="F23" r:id="rId1" xr:uid="{09DF94F6-1859-A448-B8B7-418ADFDB5F8E}"/>
+    <hyperlink ref="F24" r:id="rId2" xr:uid="{EDAF2690-88C3-BE4C-9D86-79B381B3F853}"/>
+    <hyperlink ref="F25" r:id="rId3" xr:uid="{0E9F2CCC-4F02-B845-BB59-D7E8A5B322C3}"/>
+    <hyperlink ref="F26" r:id="rId4" xr:uid="{0608EEB9-9273-034B-A2D6-21B9EE8550EE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FHIR-38108 pre-apply and CapabilityStatement fixes
</commit_message>
<xml_diff>
--- a/input/fsh/scripts/carin-bb-server.xlsx
+++ b/input/fsh/scripts/carin-bb-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cspears/dev/fhir/fsh/davinci/carin/carin-bb/input/fsh/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1208D910-C70F-3947-ACDE-20625D91DC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485C7B41-859C-FD44-A454-7ED4A2B0870E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98520" yWindow="6320" windowWidth="51200" windowHeight="28300" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-1100" windowWidth="38400" windowHeight="22380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="199">
   <si>
     <t>Element</t>
   </si>
@@ -676,10 +676,6 @@
 </t>
   </si>
   <si>
-    <t>1. See the [General Security Considerations](7_Authorization_Authentication_and_Registration.html) section for requirements and recommendations.
-1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` unauthorized response code.</t>
-  </si>
-  <si>
     <t>This Section describes the expected capabilities of the C4BB Server actor which is responsible for providing responses to the queries submitted by the C4BB Requestors. 
 The EOB Resource is the focal Consumer-Directed Payer Data Exchange (CDPDE) Resource. Several Reference Resources are defined directly/indirectly from the EOB: Coverage, Patient, Organization (Payer ID), Practioner, and Organization (Facility).
 The Coverage Reference Resource SHALL be returned with data that was effective as of the date of service of the claim; for example, the data will reflect the employer name in effect at that time. However, for other reference resources, payers MAY decide to provide either the data that was in effect as of the date of service or the current data. All reference resources within the EOB will have meta.lastUpdated flagged as must support. Payers SHALL provide the last time the data was updated or the date of creation in the payers system of record, whichever comes last. Apps will use the meta.lastUpdated values to determine if the reference resources are as of the current date or date of service.</t>
@@ -732,6 +728,19 @@
   </si>
   <si>
     <t>ExplanationOfBenefit:patient,ExplanationOfBenefit:provider,ExplanationOfBenefit:care-team,ExplanationOfBenefit:coverage,ExplanationOfBenefit:insurer,ExplanationOfBenefit:payee,ExplanationOfBenefit:*</t>
+  </si>
+  <si>
+    <t>/SearchParameter-explanationofbenefit-billable-period-start.html</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/R4/search.html#id</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/R4/search.html#lastUpdated</t>
+  </si>
+  <si>
+    <t>1. See the [General Security Considerations](Security_And_Privacy_Considerations.html) section for requirements and recommendations.
+1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` unauthorized response code.</t>
   </si>
 </sst>
 </file>
@@ -923,7 +932,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -985,6 +994,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -1416,7 +1426,7 @@
         <v>131</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1919,8 +1929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1958,7 +1968,7 @@
         <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1974,7 +1984,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2006,7 +2016,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2128,10 +2138,10 @@
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>182</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>183</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>13</v>
@@ -2252,16 +2262,16 @@
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" s="23" t="s">
         <v>191</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>192</v>
       </c>
       <c r="C12" s="23" t="s">
         <v>63</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E12" s="1" t="b">
         <v>1</v>
@@ -2407,7 +2417,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>21</v>
@@ -2416,7 +2426,7 @@
         <v>13</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="W3" s="20"/>
     </row>
@@ -2469,7 +2479,7 @@
     </row>
     <row r="7" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>63</v>
@@ -2597,7 +2607,7 @@
         <v>89</v>
       </c>
       <c r="J1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2617,7 +2627,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -2811,13 +2821,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AB32"/>
+  <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="O12" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2851,7 +2861,7 @@
     <col min="28" max="28" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -2937,7 +2947,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="13" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" s="13" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2984,7 +2994,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -3031,7 +3041,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -3079,7 +3089,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="13" customFormat="1" ht="61" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" s="13" customFormat="1" ht="61" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -3132,7 +3142,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -3179,7 +3189,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -3228,7 +3238,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -3276,7 +3286,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="78" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" ht="78" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -3293,7 +3303,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G9" t="s">
         <v>57</v>
@@ -3324,12 +3334,11 @@
       <c r="Y9" s="17"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="10"/>
-      <c r="AB9" s="1" t="str">
-        <f t="shared" ref="AB9" si="6">"SearchParameter-carin-bb-"&amp;LOWER((B9)&amp;"-"&amp;C9&amp;".html")</f>
-        <v>SearchParameter-carin-bb-explanationofbenefit-_id.html</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="78" x14ac:dyDescent="0.2">
+      <c r="AB9" s="35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="78" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f>A9+1</f>
         <v>2</v>
@@ -3347,7 +3356,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G10" t="s">
         <v>57</v>
@@ -3359,7 +3368,7 @@
         <v>69</v>
       </c>
       <c r="J10" s="1" t="str">
-        <f t="shared" ref="J10:J14" si="7">B10&amp;"."&amp;C10</f>
+        <f t="shared" ref="J10:J14" si="6">B10&amp;"."&amp;C10</f>
         <v>ExplanationOfBenefit.patient</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -3379,19 +3388,19 @@
       </c>
       <c r="X10"/>
       <c r="Y10" s="17" t="str">
-        <f t="shared" ref="Y10:Y12" si="8">"Support searching for a "&amp; B9 &amp;" by its " &amp; C10</f>
+        <f t="shared" ref="Y10:Y12" si="7">"Support searching for a "&amp; B9 &amp;" by its " &amp; C10</f>
         <v>Support searching for a ExplanationOfBenefit by its patient</v>
       </c>
       <c r="Z10" s="5"/>
       <c r="AA10" s="10"/>
       <c r="AB10" s="1" t="str">
-        <f>"SearchParameter-carin-bb-"&amp;LOWER((B10)&amp;"-"&amp;C10&amp;".html")</f>
-        <v>SearchParameter-carin-bb-explanationofbenefit-patient.html</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" ht="78" x14ac:dyDescent="0.2">
+        <f>"SearchParameter-"&amp;LOWER((B10)&amp;"-"&amp;C10&amp;".html")</f>
+        <v>SearchParameter-explanationofbenefit-patient.html</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="78" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <f t="shared" ref="A11:A21" si="9">A10+1</f>
+        <f t="shared" ref="A11:A21" si="8">A10+1</f>
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -3401,13 +3410,13 @@
         <v>141</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="E11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G11" t="s">
         <v>57</v>
@@ -3419,7 +3428,7 @@
         <v>64</v>
       </c>
       <c r="J11" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>ExplanationOfBenefit._lastUpdated</v>
       </c>
       <c r="K11" s="1" t="s">
@@ -3437,19 +3446,18 @@
       </c>
       <c r="X11"/>
       <c r="Y11" s="17" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>Support searching for a ExplanationOfBenefit by its _lastUpdated</v>
       </c>
       <c r="Z11" s="5"/>
       <c r="AA11" s="10"/>
-      <c r="AB11" s="1" t="str">
-        <f t="shared" ref="AB11:AB21" si="10">"SearchParameter-carin-bb-"&amp;LOWER((B11)&amp;"-"&amp;C11&amp;".html")</f>
-        <v>SearchParameter-carin-bb-explanationofbenefit-_lastupdated.html</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" ht="78" x14ac:dyDescent="0.2">
+      <c r="AB11" s="35" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="78" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -3465,7 +3473,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G12" t="s">
         <v>57</v>
@@ -3493,18 +3501,19 @@
         <v>13</v>
       </c>
       <c r="Y12" s="17" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>Support searching for a ExplanationOfBenefit by its type</v>
       </c>
       <c r="AA12" s="10"/>
       <c r="AB12" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-explanationofbenefit-type.html</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
+        <f t="shared" ref="AB12:AB21" si="9">"SearchParameter-"&amp;LOWER((B12)&amp;"-"&amp;C12&amp;".html")</f>
+        <v>SearchParameter-explanationofbenefit-type.html</v>
+      </c>
+      <c r="AD12" s="1"/>
+    </row>
+    <row r="13" spans="1:31" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3520,7 +3529,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>57</v>
@@ -3532,7 +3541,7 @@
         <v>58</v>
       </c>
       <c r="J13" s="1" t="str">
-        <f t="shared" ref="J13" si="11">B13&amp;"."&amp;C13</f>
+        <f t="shared" ref="J13" si="10">B13&amp;"."&amp;C13</f>
         <v>ExplanationOfBenefit.identifier</v>
       </c>
       <c r="K13" s="1" t="s">
@@ -3548,18 +3557,18 @@
         <v>13</v>
       </c>
       <c r="Y13" s="17" t="str">
-        <f t="shared" ref="Y13" si="12">"Support searching for a "&amp; B12 &amp;" by its " &amp; C13</f>
+        <f t="shared" ref="Y13" si="11">"Support searching for a "&amp; B12 &amp;" by its " &amp; C13</f>
         <v>Support searching for a ExplanationOfBenefit by its identifier</v>
       </c>
       <c r="AA13" s="10"/>
       <c r="AB13" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-explanationofbenefit-identifier.html</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" ht="78" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>SearchParameter-explanationofbenefit-identifier.html</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="78" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -3575,7 +3584,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G14" t="s">
         <v>57</v>
@@ -3587,7 +3596,7 @@
         <v>64</v>
       </c>
       <c r="J14" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>ExplanationOfBenefit.service-date</v>
       </c>
       <c r="K14" s="1" t="s">
@@ -3608,20 +3617,21 @@
       </c>
       <c r="Z14" s="5"/>
       <c r="AB14" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-explanationofbenefit-service-date.html</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>SearchParameter-explanationofbenefit-service-date.html</v>
+      </c>
+      <c r="AD14" s="1"/>
+    </row>
+    <row r="15" spans="1:31" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -3630,7 +3640,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>57</v>
@@ -3642,7 +3652,7 @@
         <v>64</v>
       </c>
       <c r="J15" s="1" t="str">
-        <f t="shared" ref="J15" si="13">B15&amp;"."&amp;C15</f>
+        <f t="shared" ref="J15" si="12">B15&amp;"."&amp;C15</f>
         <v>ExplanationOfBenefit.service-start-date</v>
       </c>
       <c r="K15" s="1" t="s">
@@ -3664,20 +3674,20 @@
       <c r="Z15" s="5"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="1" t="str">
-        <f t="shared" ref="AB15" si="14">"SearchParameter-carin-bb-"&amp;LOWER((B15)&amp;"-"&amp;C15&amp;".html")</f>
-        <v>SearchParameter-carin-bb-explanationofbenefit-service-start-date.html</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>SearchParameter-explanationofbenefit-service-start-date.html</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -3686,7 +3696,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>57</v>
@@ -3720,8 +3730,11 @@
       <c r="Z16" s="5"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="1" t="str">
-        <f t="shared" ref="AB16" si="15">"SearchParameter-carin-bb-"&amp;LOWER((B16)&amp;"-"&amp;C16&amp;".html")</f>
-        <v>SearchParameter-carin-bb-explanationofbenefit-billable-period-start.html</v>
+        <f t="shared" si="9"/>
+        <v>SearchParameter-explanationofbenefit-billable-period-start.html</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
@@ -3742,7 +3755,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>57</v>
@@ -3754,7 +3767,7 @@
         <v>69</v>
       </c>
       <c r="J17" s="1" t="str">
-        <f t="shared" ref="J17:J21" si="16">B17&amp;"."&amp;C17</f>
+        <f t="shared" ref="J17:J20" si="13">B17&amp;"."&amp;C17</f>
         <v>!ExplanationOfBenefit.provider</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -3776,13 +3789,13 @@
       <c r="Z17" s="5"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-!explanationofbenefit-provider.html</v>
+        <f t="shared" si="9"/>
+        <v>SearchParameter-!explanationofbenefit-provider.html</v>
       </c>
     </row>
     <row r="18" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -3798,7 +3811,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
@@ -3810,7 +3823,7 @@
         <v>69</v>
       </c>
       <c r="J18" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>!ExplanationOfBenefit.care-team</v>
       </c>
       <c r="K18" s="1" t="s">
@@ -3832,13 +3845,13 @@
       <c r="Z18" s="5"/>
       <c r="AA18" s="2"/>
       <c r="AB18" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-!explanationofbenefit-care-team.html</v>
+        <f t="shared" si="9"/>
+        <v>SearchParameter-!explanationofbenefit-care-team.html</v>
       </c>
     </row>
     <row r="19" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -3854,7 +3867,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>57</v>
@@ -3866,7 +3879,7 @@
         <v>69</v>
       </c>
       <c r="J19" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>!ExplanationOfBenefit.insurer</v>
       </c>
       <c r="K19" s="1" t="s">
@@ -3882,19 +3895,19 @@
         <v>13</v>
       </c>
       <c r="Y19" s="17" t="str">
-        <f t="shared" ref="Y19:Y21" si="17">"Support searching for a "&amp; B17 &amp;" by its " &amp; C19</f>
+        <f t="shared" ref="Y19:Y21" si="14">"Support searching for a "&amp; B17 &amp;" by its " &amp; C19</f>
         <v>Support searching for a !ExplanationOfBenefit by its insurer</v>
       </c>
       <c r="Z19" s="5"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-!explanationofbenefit-insurer.html</v>
+        <f t="shared" si="9"/>
+        <v>SearchParameter-!explanationofbenefit-insurer.html</v>
       </c>
     </row>
     <row r="20" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -3910,7 +3923,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>57</v>
@@ -3922,7 +3935,7 @@
         <v>69</v>
       </c>
       <c r="J20" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>!ExplanationOfBenefit.facility</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -3938,19 +3951,19 @@
         <v>13</v>
       </c>
       <c r="Y20" s="17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>Support searching for a !ExplanationOfBenefit by its facility</v>
       </c>
       <c r="Z20" s="5"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-!explanationofbenefit-facility.html</v>
+        <f t="shared" si="9"/>
+        <v>SearchParameter-!explanationofbenefit-facility.html</v>
       </c>
     </row>
     <row r="21" spans="1:28" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3966,7 +3979,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>57</v>
@@ -3994,14 +4007,14 @@
         <v>13</v>
       </c>
       <c r="Y21" s="17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>Support searching for a !ExplanationOfBenefit by its coverage</v>
       </c>
       <c r="Z21" s="5"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-!explanationofbenefit-coverage.html</v>
+        <f t="shared" si="9"/>
+        <v>SearchParameter-!explanationofbenefit-coverage.html</v>
       </c>
     </row>
     <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -4050,29 +4063,29 @@
         <v>13</v>
       </c>
       <c r="Y22" s="17"/>
-      <c r="AB22" s="1" t="str">
-        <f>"SearchParameter-carin-bb-"&amp;LOWER((B22)&amp;"-"&amp;C22&amp;".html")</f>
-        <v>SearchParameter-carin-bb-coverage-_id.html</v>
+      <c r="AB22" s="35" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
+        <f>A22+1</f>
         <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="E23" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>176</v>
+      <c r="F23" s="33" t="s">
+        <v>168</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>57</v>
@@ -4081,11 +4094,11 @@
         <v>153</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="J23" s="1" t="str">
-        <f>B23&amp;"."&amp;"id"</f>
-        <v>Patient.id</v>
+        <f>B23&amp;"."&amp;"meta.lastUpdate"</f>
+        <v>Coverage.meta.lastUpdate</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>57</v>
@@ -4101,17 +4114,16 @@
       </c>
       <c r="Y23" s="17"/>
       <c r="AA23" s="2"/>
-      <c r="AB23" s="1" t="str">
-        <f>"SearchParameter-carin-bb-"&amp;LOWER((B23)&amp;"-"&amp;C23&amp;".html")</f>
-        <v>SearchParameter-carin-bb-patient-_id.html</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB23" s="35" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>139</v>
@@ -4123,7 +4135,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>57</v>
@@ -4135,8 +4147,8 @@
         <v>58</v>
       </c>
       <c r="J24" s="1" t="str">
-        <f t="shared" ref="J24:J26" si="18">B24&amp;"."&amp;"id"</f>
-        <v>Organization.id</v>
+        <f>B24&amp;"."&amp;"id"</f>
+        <v>Patient.id</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>57</v>
@@ -4145,26 +4157,26 @@
         <v>57</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="Y24" s="17"/>
-      <c r="AB24" s="1" t="str">
-        <f t="shared" ref="AB24:AB26" si="19">"SearchParameter-carin-bb-"&amp;LOWER((B24)&amp;"-"&amp;C24&amp;".html")</f>
-        <v>SearchParameter-carin-bb-organization-_id.html</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>63</v>
@@ -4173,7 +4185,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>57</v>
@@ -4182,11 +4194,11 @@
         <v>153</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="J25" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>Practitioner.id</v>
+        <f>B25&amp;"."&amp;"meta.lastUpdate"</f>
+        <v>Patient.meta.lastUpdate</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>57</v>
@@ -4195,23 +4207,23 @@
         <v>57</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="Y25" s="17"/>
-      <c r="AB25" s="1" t="str">
-        <f t="shared" si="19"/>
-        <v>SearchParameter-carin-bb-practitioner-_id.html</v>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="35" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>193</v>
+        <v>84</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>139</v>
@@ -4223,7 +4235,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>57</v>
@@ -4235,8 +4247,8 @@
         <v>58</v>
       </c>
       <c r="J26" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>RelatedPerson.id</v>
+        <f t="shared" ref="J26:J30" si="15">B26&amp;"."&amp;"id"</f>
+        <v>Organization.id</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>57</v>
@@ -4251,45 +4263,257 @@
         <v>63</v>
       </c>
       <c r="Y26" s="17"/>
-      <c r="AB26" s="1" t="str">
-        <f t="shared" si="19"/>
-        <v>SearchParameter-carin-bb-relatedperson-_id.html</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="AB26" s="35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>14</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="1" t="str">
+        <f>B27&amp;"."&amp;"meta.lastUpdate"</f>
+        <v>Organization.meta.lastUpdate</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="Y27" s="17"/>
-      <c r="AB27" s="1"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="35" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="A28" s="1">
+        <v>15</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J28" s="1" t="str">
+        <f t="shared" si="15"/>
+        <v>Practitioner.id</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="Y28" s="17"/>
-      <c r="AB28" s="1"/>
-    </row>
-    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="AB28" s="35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>15</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" s="1" t="str">
+        <f>B29&amp;"."&amp;"meta.lastUpdate"</f>
+        <v>Practitioner.meta.lastUpdate</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="Y29" s="17"/>
-      <c r="AB29" s="1"/>
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="35" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="A30" s="1">
+        <v>16</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J30" s="1" t="str">
+        <f t="shared" si="15"/>
+        <v>RelatedPerson.id</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="Y30" s="17"/>
-      <c r="AB30" s="1"/>
-    </row>
-    <row r="31" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="AB30" s="35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>16</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J31" s="1" t="str">
+        <f>B31&amp;"."&amp;"meta.lastUpdate"</f>
+        <v>RelatedPerson.meta.lastUpdate</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="Y31" s="17"/>
-      <c r="AB31" s="1"/>
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="35" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="32" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G32" s="1"/>
@@ -4298,19 +4522,66 @@
       <c r="Y32" s="17"/>
       <c r="AB32" s="1"/>
     </row>
+    <row r="33" spans="7:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="Y33" s="17"/>
+      <c r="AB33" s="1"/>
+    </row>
+    <row r="34" spans="7:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="Y34" s="17"/>
+      <c r="AB34" s="1"/>
+    </row>
+    <row r="35" spans="7:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="Y35" s="17"/>
+      <c r="AB35" s="1"/>
+    </row>
+    <row r="36" spans="7:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="Y36" s="17"/>
+      <c r="AB36" s="1"/>
+    </row>
+    <row r="37" spans="7:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="Y37" s="17"/>
+      <c r="AB37" s="1"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AB21" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA21">
     <sortCondition ref="B1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F23" r:id="rId1" xr:uid="{09DF94F6-1859-A448-B8B7-418ADFDB5F8E}"/>
-    <hyperlink ref="F24" r:id="rId2" xr:uid="{EDAF2690-88C3-BE4C-9D86-79B381B3F853}"/>
-    <hyperlink ref="F25" r:id="rId3" xr:uid="{0E9F2CCC-4F02-B845-BB59-D7E8A5B322C3}"/>
-    <hyperlink ref="F26" r:id="rId4" xr:uid="{0608EEB9-9273-034B-A2D6-21B9EE8550EE}"/>
+    <hyperlink ref="F24" r:id="rId1" xr:uid="{09DF94F6-1859-A448-B8B7-418ADFDB5F8E}"/>
+    <hyperlink ref="F26" r:id="rId2" xr:uid="{EDAF2690-88C3-BE4C-9D86-79B381B3F853}"/>
+    <hyperlink ref="F28" r:id="rId3" xr:uid="{0E9F2CCC-4F02-B845-BB59-D7E8A5B322C3}"/>
+    <hyperlink ref="F30" r:id="rId4" xr:uid="{0608EEB9-9273-034B-A2D6-21B9EE8550EE}"/>
+    <hyperlink ref="AB9" r:id="rId5" location="id" xr:uid="{3A427A9E-F6F9-6649-8484-2662A4F9148C}"/>
+    <hyperlink ref="AB22" r:id="rId6" location="id" xr:uid="{DD7D12F6-4F92-7D47-8DC4-514667945F2C}"/>
+    <hyperlink ref="AB11" r:id="rId7" location="lastUpdated" xr:uid="{4E353ADA-DEF5-0349-8995-D052CC33521C}"/>
+    <hyperlink ref="F25" r:id="rId8" xr:uid="{8CBCC217-6B3F-9944-9B85-D12E096AA01C}"/>
+    <hyperlink ref="F27" r:id="rId9" xr:uid="{50639181-8A32-9444-9409-E625280C229F}"/>
+    <hyperlink ref="F29" r:id="rId10" xr:uid="{25FC2AF6-E699-AE44-BBF0-A3C97A75C3E5}"/>
+    <hyperlink ref="F31" r:id="rId11" xr:uid="{1B5AA4E8-734C-CC4D-9C4C-72B7EBF5768C}"/>
+    <hyperlink ref="AB23" r:id="rId12" location="lastUpdated" xr:uid="{37557FBB-3B01-F94E-804F-DE8A58CE763C}"/>
+    <hyperlink ref="AB25" r:id="rId13" location="lastUpdated" xr:uid="{4EC307BB-8900-9A45-8B97-1EFF21EF3B22}"/>
+    <hyperlink ref="AB27" r:id="rId14" location="lastUpdated" xr:uid="{80E3DA0E-11B3-7E49-AD78-328924CA27CB}"/>
+    <hyperlink ref="AB29" r:id="rId15" location="lastUpdated" xr:uid="{16B31A2F-A796-9741-9324-87ADCA30DC3A}"/>
+    <hyperlink ref="AB31" r:id="rId16" location="lastUpdated" xr:uid="{8AD4C8C7-21A1-6B4F-B8C7-ABEC7A9A20BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId17"/>
+  <legacyDrawing r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>